<commit_message>
Paper revision June 2021
</commit_message>
<xml_diff>
--- a/datasets/targetCrops_europe.xlsx
+++ b/datasets/targetCrops_europe.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="189">
   <si>
     <t>crops</t>
   </si>
@@ -583,90 +583,6 @@
   </si>
   <si>
     <t>Fallow land</t>
-  </si>
-  <si>
-    <t>J0000</t>
-  </si>
-  <si>
-    <t>Permanent grassland</t>
-  </si>
-  <si>
-    <t>PECR</t>
-  </si>
-  <si>
-    <t>Permanent crops</t>
-  </si>
-  <si>
-    <t>F0000</t>
-  </si>
-  <si>
-    <t>Fruits, berries and nuts (excluding citrus fruits, grapes and strawberries)</t>
-  </si>
-  <si>
-    <t>FRUIT NES FRESH</t>
-  </si>
-  <si>
-    <t>fruit</t>
-  </si>
-  <si>
-    <t>perennial</t>
-  </si>
-  <si>
-    <t>tree</t>
-  </si>
-  <si>
-    <t>T0000</t>
-  </si>
-  <si>
-    <t>Citrus fruits</t>
-  </si>
-  <si>
-    <t>CITRUS FRUIT NES</t>
-  </si>
-  <si>
-    <t>W1000</t>
-  </si>
-  <si>
-    <t>Grapes</t>
-  </si>
-  <si>
-    <t>GRAPES</t>
-  </si>
-  <si>
-    <t>shrub</t>
-  </si>
-  <si>
-    <t>O1000</t>
-  </si>
-  <si>
-    <t>Olives</t>
-  </si>
-  <si>
-    <t>OLIVES</t>
-  </si>
-  <si>
-    <t>H9000</t>
-  </si>
-  <si>
-    <t>Other permanent crops for human consumption n.e.c.</t>
-  </si>
-  <si>
-    <t>L0000</t>
-  </si>
-  <si>
-    <t>Nurseries</t>
-  </si>
-  <si>
-    <t>PECR9</t>
-  </si>
-  <si>
-    <t>Other permanent crops</t>
-  </si>
-  <si>
-    <t>K0000</t>
-  </si>
-  <si>
-    <t>Kitchen gardens</t>
   </si>
   <si>
     <t>Mean</t>
@@ -1476,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2184,7 +2100,7 @@
         <v>36666.666669999999</v>
       </c>
       <c r="G23" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="H23" t="s">
         <v>26</v>
@@ -3649,314 +3565,6 @@
         <v>12</v>
       </c>
       <c r="J70" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>188</v>
-      </c>
-      <c r="B71" t="s">
-        <v>189</v>
-      </c>
-      <c r="C71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71" t="s">
-        <v>12</v>
-      </c>
-      <c r="F71" t="s">
-        <v>12</v>
-      </c>
-      <c r="G71" t="s">
-        <v>13</v>
-      </c>
-      <c r="H71" t="s">
-        <v>12</v>
-      </c>
-      <c r="I71" t="s">
-        <v>12</v>
-      </c>
-      <c r="J71" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>190</v>
-      </c>
-      <c r="B72" t="s">
-        <v>191</v>
-      </c>
-      <c r="C72" t="s">
-        <v>12</v>
-      </c>
-      <c r="D72" t="s">
-        <v>12</v>
-      </c>
-      <c r="E72" t="s">
-        <v>12</v>
-      </c>
-      <c r="F72" t="s">
-        <v>12</v>
-      </c>
-      <c r="G72" t="s">
-        <v>138</v>
-      </c>
-      <c r="H72" t="s">
-        <v>12</v>
-      </c>
-      <c r="I72" t="s">
-        <v>12</v>
-      </c>
-      <c r="J72" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>192</v>
-      </c>
-      <c r="B73" t="s">
-        <v>193</v>
-      </c>
-      <c r="C73" t="s">
-        <v>194</v>
-      </c>
-      <c r="D73">
-        <v>450000</v>
-      </c>
-      <c r="E73">
-        <v>5000</v>
-      </c>
-      <c r="F73">
-        <v>5000</v>
-      </c>
-      <c r="H73" t="s">
-        <v>195</v>
-      </c>
-      <c r="I73" t="s">
-        <v>196</v>
-      </c>
-      <c r="J73" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>198</v>
-      </c>
-      <c r="B74" t="s">
-        <v>199</v>
-      </c>
-      <c r="C74" t="s">
-        <v>200</v>
-      </c>
-      <c r="D74">
-        <v>260000</v>
-      </c>
-      <c r="E74">
-        <v>5000</v>
-      </c>
-      <c r="F74">
-        <v>2000</v>
-      </c>
-      <c r="H74" t="s">
-        <v>195</v>
-      </c>
-      <c r="I74" t="s">
-        <v>196</v>
-      </c>
-      <c r="J74" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>201</v>
-      </c>
-      <c r="B75" t="s">
-        <v>202</v>
-      </c>
-      <c r="C75" t="s">
-        <v>203</v>
-      </c>
-      <c r="D75">
-        <v>530000</v>
-      </c>
-      <c r="E75">
-        <v>5000</v>
-      </c>
-      <c r="F75">
-        <v>4000</v>
-      </c>
-      <c r="H75" t="s">
-        <v>195</v>
-      </c>
-      <c r="I75" t="s">
-        <v>196</v>
-      </c>
-      <c r="J75" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>205</v>
-      </c>
-      <c r="B76" t="s">
-        <v>206</v>
-      </c>
-      <c r="C76" t="s">
-        <v>207</v>
-      </c>
-      <c r="D76">
-        <v>1750000</v>
-      </c>
-      <c r="E76">
-        <v>13000</v>
-      </c>
-      <c r="F76">
-        <v>175000</v>
-      </c>
-      <c r="H76" t="s">
-        <v>115</v>
-      </c>
-      <c r="I76" t="s">
-        <v>196</v>
-      </c>
-      <c r="J76" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>208</v>
-      </c>
-      <c r="B77" t="s">
-        <v>209</v>
-      </c>
-      <c r="C77" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" t="s">
-        <v>12</v>
-      </c>
-      <c r="F77" t="s">
-        <v>12</v>
-      </c>
-      <c r="G77" t="s">
-        <v>138</v>
-      </c>
-      <c r="H77" t="s">
-        <v>12</v>
-      </c>
-      <c r="I77" t="s">
-        <v>12</v>
-      </c>
-      <c r="J77" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>210</v>
-      </c>
-      <c r="B78" t="s">
-        <v>211</v>
-      </c>
-      <c r="C78" t="s">
-        <v>12</v>
-      </c>
-      <c r="D78" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" t="s">
-        <v>12</v>
-      </c>
-      <c r="F78" t="s">
-        <v>12</v>
-      </c>
-      <c r="G78" t="s">
-        <v>13</v>
-      </c>
-      <c r="H78" t="s">
-        <v>12</v>
-      </c>
-      <c r="I78" t="s">
-        <v>12</v>
-      </c>
-      <c r="J78" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>212</v>
-      </c>
-      <c r="B79" t="s">
-        <v>213</v>
-      </c>
-      <c r="C79" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" t="s">
-        <v>12</v>
-      </c>
-      <c r="F79" t="s">
-        <v>12</v>
-      </c>
-      <c r="G79" t="s">
-        <v>138</v>
-      </c>
-      <c r="H79" t="s">
-        <v>12</v>
-      </c>
-      <c r="I79" t="s">
-        <v>12</v>
-      </c>
-      <c r="J79" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>214</v>
-      </c>
-      <c r="B80" t="s">
-        <v>215</v>
-      </c>
-      <c r="C80" t="s">
-        <v>12</v>
-      </c>
-      <c r="D80" t="s">
-        <v>12</v>
-      </c>
-      <c r="E80" t="s">
-        <v>12</v>
-      </c>
-      <c r="F80" t="s">
-        <v>12</v>
-      </c>
-      <c r="G80" t="s">
-        <v>138</v>
-      </c>
-      <c r="H80" t="s">
-        <v>12</v>
-      </c>
-      <c r="I80" t="s">
-        <v>12</v>
-      </c>
-      <c r="J80" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>